<commit_message>
indention of annotation label
</commit_message>
<xml_diff>
--- a/inst/extdata/ANNOTATION_TEMPLATE.xlsx
+++ b/inst/extdata/ANNOTATION_TEMPLATE.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989"/>
   </bookViews>
   <sheets>
-    <sheet name="ANNOTATION_TEMPLATE" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ANNOTATION_TEMPLATE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="53">
   <si>
     <t>PROJECT</t>
   </si>
@@ -168,38 +167,37 @@
   </si>
   <si>
     <t>Orchidaceae</t>
+  </si>
+  <si>
+    <t>Orchidaceae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Updated the family according to APGIII</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,7 +209,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -219,80 +217,340 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:S22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="14" min="1" style="1" width="8.05668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="21.7368421052632"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.05668016194332"/>
+    <col min="1" max="14" width="8" style="1"/>
+    <col min="15" max="15" width="21.77734375" style="1"/>
+    <col min="16" max="1025" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -351,7 +609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -361,7 +619,7 @@
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="0"/>
+      <c r="D2"/>
       <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
@@ -389,17 +647,17 @@
       <c r="R2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="2" t="n">
+      <c r="S2" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:19">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
       <c r="F3" s="2" t="s">
         <v>31</v>
       </c>
@@ -421,21 +679,21 @@
       <c r="O3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="0"/>
+      <c r="P3"/>
       <c r="R3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="2" t="n">
+      <c r="S3" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
       <c r="F4" s="2" t="s">
         <v>36</v>
       </c>
@@ -457,21 +715,21 @@
       <c r="O4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="0"/>
+      <c r="P4"/>
       <c r="R4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="2" t="n">
+      <c r="S4" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
       <c r="F5" s="2" t="s">
         <v>39</v>
       </c>
@@ -493,20 +751,20 @@
       <c r="O5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="0"/>
-      <c r="R5" s="0"/>
-      <c r="S5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
       <c r="L6" s="2" t="s">
         <v>25</v>
       </c>
@@ -517,23 +775,23 @@
       <c r="O6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="0"/>
+      <c r="P6"/>
       <c r="R6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S6" s="2" t="n">
+      <c r="S6" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
+    <row r="7" spans="1:19">
+      <c r="A7"/>
       <c r="B7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="0"/>
+      <c r="D7"/>
       <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
@@ -553,19 +811,19 @@
       <c r="O7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P7" s="0"/>
-      <c r="R7" s="0"/>
-      <c r="S7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
+      <c r="P7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8"/>
       <c r="B8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="0"/>
+      <c r="D8"/>
       <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
@@ -585,19 +843,19 @@
       <c r="O8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="0"/>
-      <c r="R8" s="0"/>
-      <c r="S8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0"/>
+      <c r="P8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9"/>
       <c r="B9" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="0"/>
+      <c r="D9"/>
       <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
@@ -617,21 +875,21 @@
       <c r="O9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P9" s="0"/>
+      <c r="P9"/>
       <c r="R9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S9" s="2" t="n">
+      <c r="S9" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
@@ -653,19 +911,19 @@
       <c r="O10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P10" s="0"/>
-      <c r="R10" s="0"/>
-      <c r="S10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
+      <c r="P10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="0"/>
+      <c r="D11"/>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
@@ -687,19 +945,19 @@
       <c r="O11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="0"/>
+      <c r="P11"/>
       <c r="R11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S11" s="2" t="n">
+      <c r="S11" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:19">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="0"/>
+      <c r="D12"/>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
@@ -721,15 +979,15 @@
       <c r="O12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="0"/>
-      <c r="R12" s="0"/>
-      <c r="S12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="0"/>
+      <c r="D13"/>
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
@@ -751,16 +1009,16 @@
       <c r="O13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="0"/>
+      <c r="P13"/>
       <c r="R13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S13" s="2" t="n">
+      <c r="S13" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="0"/>
+    <row r="14" spans="1:19">
+      <c r="D14"/>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
@@ -773,24 +1031,24 @@
       <c r="L14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="0"/>
+      <c r="M14"/>
       <c r="N14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="0"/>
-      <c r="R14" s="0"/>
-      <c r="S14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
       <c r="L15" s="2" t="s">
         <v>25</v>
       </c>
@@ -809,17 +1067,17 @@
       <c r="R15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S15" s="2" t="n">
+      <c r="S15" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:19">
       <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="0"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="L16" s="2" t="s">
         <v>25</v>
       </c>
@@ -838,14 +1096,14 @@
       <c r="R16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S16" s="2" t="n">
+      <c r="S16" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="0"/>
-      <c r="G17" s="0"/>
-      <c r="H17" s="0"/>
+    <row r="17" spans="4:19">
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="L17" s="2" t="s">
         <v>25</v>
       </c>
@@ -861,13 +1119,13 @@
       <c r="P17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R17" s="0"/>
-      <c r="S17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
+      <c r="R17"/>
+      <c r="S17"/>
+    </row>
+    <row r="18" spans="4:19">
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
       <c r="L18" s="2" t="s">
         <v>25</v>
       </c>
@@ -880,14 +1138,14 @@
       <c r="O18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P18" s="0"/>
-      <c r="R18" s="0"/>
-      <c r="S18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
+      <c r="P18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+    </row>
+    <row r="19" spans="4:19">
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
       <c r="L19" s="2" t="s">
         <v>25</v>
       </c>
@@ -903,13 +1161,13 @@
       <c r="P19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R19" s="0"/>
-      <c r="S19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="0"/>
-      <c r="G20" s="0"/>
-      <c r="H20" s="0"/>
+      <c r="R19"/>
+      <c r="S19"/>
+    </row>
+    <row r="20" spans="4:19">
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
       <c r="L20" s="2" t="s">
         <v>25</v>
       </c>
@@ -928,14 +1186,14 @@
       <c r="R20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S20" s="2" t="n">
+      <c r="S20" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
-      <c r="H21" s="0"/>
+    <row r="21" spans="4:19">
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="L21" s="2" t="s">
         <v>25</v>
       </c>
@@ -948,10 +1206,10 @@
       <c r="O21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="R21" s="0"/>
-      <c r="S21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R21"/>
+      <c r="S21"/>
+    </row>
+    <row r="22" spans="4:19">
       <c r="F22" s="2" t="s">
         <v>22</v>
       </c>
@@ -970,17 +1228,42 @@
       <c r="R22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S22" s="2" t="n">
+      <c r="S22" s="2">
         <v>224</v>
       </c>
     </row>
+    <row r="23" spans="4:19">
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="L23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S23" s="2">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>